<commit_message>
changing exp names in ESA_231218
</commit_message>
<xml_diff>
--- a/scripts-ESA/ESA_231218.xlsx
+++ b/scripts-ESA/ESA_231218.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au583430_uni_au_dk/Documents/Documents/GitHub/Pedersen-2023-sep-and-plasma-treat/scripts-ESA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D07A0E56-E32D-4706-B083-9D758B20E785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{D07A0E56-E32D-4706-B083-9D758B20E785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5582A728-A599-413F-9BFC-2981A3C0ECDE}"/>
   <bookViews>
-    <workbookView xWindow="-33645" yWindow="1830" windowWidth="28800" windowHeight="16515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33645" yWindow="1830" windowWidth="28800" windowHeight="16515" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InitialValue" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="60">
   <si>
     <t>Levels</t>
   </si>
@@ -118,18 +118,6 @@
   </si>
   <si>
     <t>9.49(8.26-10.72)a</t>
-  </si>
-  <si>
-    <t>22H</t>
-  </si>
-  <si>
-    <t>22I</t>
-  </si>
-  <si>
-    <t>22J</t>
-  </si>
-  <si>
-    <t>22K</t>
   </si>
   <si>
     <t>0.92(0.28-1.56)a</t>
@@ -567,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +585,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -608,7 +596,7 @@
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -619,7 +607,7 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -630,7 +618,7 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -641,7 +629,7 @@
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,7 +640,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -674,7 +662,7 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -685,7 +673,7 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -696,7 +684,7 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,7 +695,7 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -718,7 +706,7 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -730,7 +718,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D3:D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -767,10 +757,10 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -781,10 +771,10 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -795,10 +785,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -809,10 +799,10 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -823,10 +813,10 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -837,10 +827,10 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -851,10 +841,10 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -865,10 +855,10 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -879,10 +869,10 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,10 +883,10 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -907,10 +897,10 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,10 +911,10 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +926,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -959,10 +951,10 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -973,10 +965,10 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,10 +979,10 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1001,10 +993,10 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1015,10 +1007,10 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1029,10 +1021,10 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1043,10 +1035,10 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1057,10 +1049,10 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1071,10 +1063,10 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1085,10 +1077,10 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1099,10 +1091,10 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1113,10 +1105,10 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
         <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updating ESA data with correct exp key
</commit_message>
<xml_diff>
--- a/scripts-ESA/ESA_231218.xlsx
+++ b/scripts-ESA/ESA_231218.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au583430_uni_au_dk/Documents/Documents/GitHub/Pedersen-2023-sep-and-plasma-treat/scripts-ESA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{D07A0E56-E32D-4706-B083-9D758B20E785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5582A728-A599-413F-9BFC-2981A3C0ECDE}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{D07A0E56-E32D-4706-B083-9D758B20E785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{351F4787-77F6-423B-96C3-D5F5F276FBC5}"/>
   <bookViews>
-    <workbookView xWindow="-33645" yWindow="1830" windowWidth="28800" windowHeight="16515" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31650" yWindow="3150" windowWidth="28800" windowHeight="16515" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InitialValue" sheetId="1" r:id="rId1"/>
@@ -927,10 +927,15 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D13"/>
+      <selection activeCell="D10" sqref="C8:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">

</xml_diff>